<commit_message>
Empleado: Apartado otros finalizado parcialmente
</commit_message>
<xml_diff>
--- a/rh-admin/adm/modelos/modelos tablas.xlsx
+++ b/rh-admin/adm/modelos/modelos tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulsa\Desktop\rh-admin\rh-admin\adm\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEEB329-88E5-4E2E-9A1B-8E81D7889898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C7214A-D038-493D-A57D-9D2BC5C200FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-600" windowWidth="29040" windowHeight="15720" xr2:uid="{C2718D48-A303-4290-B486-461D75A79B03}"/>
   </bookViews>
@@ -292,10 +292,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B2BE8F-DD3E-4494-B8DD-52782E64F77B}">
   <dimension ref="A5:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,8 +644,8 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="F6" t="s">
         <v>47</v>
       </c>
@@ -797,13 +797,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
vacaciones y suspensiones con sus acciones
</commit_message>
<xml_diff>
--- a/rh-admin/adm/modelos/modelos tablas.xlsx
+++ b/rh-admin/adm/modelos/modelos tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulsa\Desktop\rh-admin\rh-admin\adm\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C7214A-D038-493D-A57D-9D2BC5C200FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD6376A-3E0D-4225-851D-5EC992F2D263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-600" windowWidth="29040" windowHeight="15720" xr2:uid="{C2718D48-A303-4290-B486-461D75A79B03}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>UPDATABLE_DOCUMENTS</t>
+  </si>
+  <si>
+    <t>DIPLOMAS</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B2BE8F-DD3E-4494-B8DD-52782E64F77B}">
-  <dimension ref="A5:O30"/>
+  <dimension ref="A5:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,11 +625,11 @@
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -636,11 +639,11 @@
       <c r="I5" t="s">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -650,19 +653,19 @@
         <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -673,20 +676,21 @@
       <c r="G7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="K7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="O7" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>48</v>
       </c>
@@ -694,105 +698,107 @@
         <v>25</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="O8" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="J9" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="J10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="J11" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>52</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -906,9 +912,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>